<commit_message>
Added Second exam topics
</commit_message>
<xml_diff>
--- a/Parcial 2/02 Tablas dinamicas/02 Datos de Cosechas.xlsx
+++ b/Parcial 2/02 Tablas dinamicas/02 Datos de Cosechas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARIAMONICA\Documents\ITAM\ITAM-CURSOS\COMPU II\EXCEL\EXCEL AVANZADO\TABLAS DINAMICAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmond\Documents\ITAM\Semestre 10\Herramientas Computacionales para Produccion Empresarial\hcp-repo\Parcial 2\02 Tablas dinamicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D1584B-0DB9-432B-86E7-DAC42104DC0B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15195" windowHeight="8235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos de Cosechas" sheetId="1" r:id="rId1"/>
@@ -69,11 +70,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +83,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -108,18 +117,95 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -130,6 +216,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7D6E3A1F-9680-41F1-9D2F-87A8577863B5}" name="Tabla1" displayName="Tabla1" ref="A1:F501" totalsRowShown="0" dataDxfId="0" dataCellStyle="Millares">
+  <autoFilter ref="A1:F501" xr:uid="{71A39075-E5B2-4730-8457-EFEFDD3EF37F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{FA18D4EE-C4C0-45D0-AFE4-D6A5A99A77E6}" name="País"/>
+    <tableColumn id="2" xr3:uid="{60BAB6D6-8775-460F-8942-EF6160E9E12B}" name="Grano"/>
+    <tableColumn id="3" xr3:uid="{CB833DBA-4E98-4E2D-9D79-A51E8CC5A9BA}" name="Compras" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="4" xr3:uid="{CA26F2F1-1320-4D4B-AF4D-EFF49188F55B}" name="Ventas" dataDxfId="3" dataCellStyle="Millares"/>
+    <tableColumn id="5" xr3:uid="{340A0B5B-546F-42C3-809F-7B3C01AD17A9}" name="Solicitudes" dataDxfId="2" dataCellStyle="Millares"/>
+    <tableColumn id="6" xr3:uid="{48E3A5CA-3B85-4997-BF00-DCDE0DFF09F4}" name="Otros" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -208,6 +309,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -243,6 +361,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -418,16 +553,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F501"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="11.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -447,7 +585,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -467,7 +605,7 @@
         <v>318.62849818414867</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -487,7 +625,7 @@
         <v>-263.10007019257182</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -507,7 +645,7 @@
         <v>288.67458113345748</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -527,7 +665,7 @@
         <v>-96.514786217841106</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -547,7 +685,7 @@
         <v>163.07565538499102</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -567,7 +705,7 @@
         <v>242.0728171636097</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -587,7 +725,7 @@
         <v>-4.5167394024475698</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -607,7 +745,7 @@
         <v>43.885616626483966</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -627,7 +765,7 @@
         <v>-191.99194311349834</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -647,7 +785,7 @@
         <v>182.42439039277323</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -667,7 +805,7 @@
         <v>-295.12924588763082</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -687,7 +825,7 @@
         <v>-386.95944090090643</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -707,7 +845,7 @@
         <v>-14.2216254158147</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -727,7 +865,7 @@
         <v>71.596423230689481</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -747,7 +885,7 @@
         <v>-177.34305856501965</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -767,7 +905,7 @@
         <v>244.8805200354015</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -787,7 +925,7 @@
         <v>130.57344279305394</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -807,7 +945,7 @@
         <v>393.29203161717578</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -827,7 +965,7 @@
         <v>-327.28049562059391</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -847,7 +985,7 @@
         <v>331.17160557878356</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -867,7 +1005,7 @@
         <v>-55.284279915768906</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -886,8 +1024,9 @@
       <c r="F23" s="2">
         <v>64.897610400708032</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -907,7 +1046,7 @@
         <v>229.33133945738089</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -927,7 +1066,7 @@
         <v>3.0060731833856948</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -947,7 +1086,7 @@
         <v>156.19373149815365</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -967,7 +1106,7 @@
         <v>-266.91488387707147</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -987,7 +1126,7 @@
         <v>384.25855281228064</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1007,7 +1146,7 @@
         <v>162.63313699758908</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1166,7 @@
         <v>-94.927823725089269</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1047,7 +1186,7 @@
         <v>89.068269905697804</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1067,7 +1206,7 @@
         <v>186.94112979522077</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1226,7 @@
         <v>253.77666554765463</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1107,7 +1246,7 @@
         <v>196.47816400646994</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -1127,7 +1266,7 @@
         <v>-109.22574541459392</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1147,7 +1286,7 @@
         <v>-5.4322946867275164</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1306,7 @@
         <v>-42.359691152684093</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -1187,7 +1326,7 @@
         <v>357.2649311807611</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -1207,7 +1346,7 @@
         <v>-120.38026062807093</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1227,7 +1366,7 @@
         <v>-30.106509598071227</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +1386,7 @@
         <v>2.2888882106998096</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -1267,7 +1406,7 @@
         <v>-65.675832392345939</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1426,7 @@
         <v>-220.7708975493637</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1307,7 +1446,7 @@
         <v>-135.85314493240153</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1466,7 @@
         <v>-227.31711783196508</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1347,7 +1486,7 @@
         <v>-28.382213812677389</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -1367,7 +1506,7 @@
         <v>63.875240333262127</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1387,7 +1526,7 @@
         <v>22.751548814355914</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -1407,7 +1546,7 @@
         <v>-90.868861964781672</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -1427,7 +1566,7 @@
         <v>103.6866359447005</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -1447,7 +1586,7 @@
         <v>183.66039002655111</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1467,7 +1606,7 @@
         <v>50.981170079653324</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1487,7 +1626,7 @@
         <v>81.469161046174506</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1507,7 +1646,7 @@
         <v>-96.89626758629106</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1527,7 +1666,7 @@
         <v>-65.523239844965957</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1547,7 +1686,7 @@
         <v>77.455977050080861</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1706,7 @@
         <v>-373.60759300515764</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -1587,7 +1726,7 @@
         <v>-80.782494582964517</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -1607,7 +1746,7 @@
         <v>159.94750816370131</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1627,7 +1766,7 @@
         <v>52.735984374523127</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -1647,7 +1786,7 @@
         <v>-264.1376995147557</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -1667,7 +1806,7 @@
         <v>345.98834192938023</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -1687,7 +1826,7 @@
         <v>-27.253028962065486</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1846,7 @@
         <v>20.477919858394102</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -1727,7 +1866,7 @@
         <v>-116.48915066988127</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -1747,7 +1886,7 @@
         <v>-244.04126102481158</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1767,7 +1906,7 @@
         <v>-316.79738761558883</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +1926,7 @@
         <v>-201.04068117313153</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -1807,7 +1946,7 @@
         <v>176.93105868709375</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -1827,7 +1966,7 @@
         <v>-161.5039521469771</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>3</v>
       </c>
@@ -1847,7 +1986,7 @@
         <v>122.22663045136876</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -1867,7 +2006,7 @@
         <v>9.9948118533890806</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -1887,7 +2026,7 @@
         <v>-176.73268837549969</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -1907,7 +2046,7 @@
         <v>79.073458052308723</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -1927,7 +2066,7 @@
         <v>46.250801110873738</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -1947,7 +2086,7 @@
         <v>-106.73848689230022</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -1967,7 +2106,7 @@
         <v>-104.34278389843439</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -1987,7 +2126,7 @@
         <v>-182.36335337382127</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -2007,7 +2146,7 @@
         <v>-188.0245368816187</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -2027,7 +2166,7 @@
         <v>-156.88039796136357</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -2047,7 +2186,7 @@
         <v>87.740714743491935</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -2067,7 +2206,7 @@
         <v>123.46263008514669</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -2087,7 +2226,7 @@
         <v>7.8432569353312829</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -2107,7 +2246,7 @@
         <v>105.60930204168827</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -2127,7 +2266,7 @@
         <v>144.13892025513474</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -2147,7 +2286,7 @@
         <v>423.70372631000703</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -2167,7 +2306,7 @@
         <v>230.17059846797082</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>2</v>
       </c>
@@ -2187,7 +2326,7 @@
         <v>73.1070894497513</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -2207,7 +2346,7 @@
         <v>154.16425061799981</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -2227,7 +2366,7 @@
         <v>323.51145970030825</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -2247,7 +2386,7 @@
         <v>191.30527665028842</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -2267,7 +2406,7 @@
         <v>114.26129947813351</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -2287,7 +2426,7 @@
         <v>-103.71715445417645</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -2307,7 +2446,7 @@
         <v>-445.00564592425309</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -2327,7 +2466,7 @@
         <v>-152.6383251442</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -2347,7 +2486,7 @@
         <v>-123.61522263252664</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -2367,7 +2506,7 @@
         <v>-79.088717307046721</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -2387,7 +2526,7 @@
         <v>-7.2939237647633206</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -2407,7 +2546,7 @@
         <v>232.88674581133461</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>2</v>
       </c>
@@ -2427,7 +2566,7 @@
         <v>-1.80059205908384</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>1</v>
       </c>
@@ -2447,7 +2586,7 @@
         <v>58.931241798150573</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -2467,7 +2606,7 @@
         <v>172.73476363414414</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>3</v>
       </c>
@@ -2487,7 +2626,7 @@
         <v>190.09979552598651</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -2507,7 +2646,7 @@
         <v>-329.98138370921964</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -2527,7 +2666,7 @@
         <v>-456.51112399670399</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>2</v>
       </c>
@@ -2547,7 +2686,7 @@
         <v>-246.52851954710533</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -2567,7 +2706,7 @@
         <v>-319.80346079897458</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -2587,7 +2726,7 @@
         <v>-20.737327188940085</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -2607,7 +2746,7 @@
         <v>432.72194586016417</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>2</v>
       </c>
@@ -2627,7 +2766,7 @@
         <v>-144.62721640675068</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>3</v>
       </c>
@@ -2647,7 +2786,7 @@
         <v>364.23841059602648</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>0</v>
       </c>
@@ -2667,7 +2806,7 @@
         <v>-21.40873439741199</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -2687,7 +2826,7 @@
         <v>20.416882839442138</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>2</v>
       </c>
@@ -2707,7 +2846,7 @@
         <v>-283.30332346568196</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -2727,7 +2866,7 @@
         <v>-359.24863429670097</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>2</v>
       </c>
@@ -2747,7 +2886,7 @@
         <v>414.22772911770994</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>3</v>
       </c>
@@ -2767,7 +2906,7 @@
         <v>-77.028717917416884</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>0</v>
       </c>
@@ -2787,7 +2926,7 @@
         <v>103.64085818048648</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>1</v>
       </c>
@@ -2807,7 +2946,7 @@
         <v>-171.60557878353217</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>2</v>
       </c>
@@ -2827,7 +2966,7 @@
         <v>51.683095797601254</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>3</v>
       </c>
@@ -2847,7 +2986,7 @@
         <v>29.129917294839316</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>0</v>
       </c>
@@ -2867,7 +3006,7 @@
         <v>-88.518936735129842</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>1</v>
       </c>
@@ -2887,7 +3026,7 @@
         <v>180.19653920102536</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>2</v>
       </c>
@@ -2907,7 +3046,7 @@
         <v>37.064729758598617</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -2927,7 +3066,7 @@
         <v>0.76296273689992944</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +3086,7 @@
         <v>394.97054963835564</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>1</v>
       </c>
@@ -2967,7 +3106,7 @@
         <v>-82.522049623096393</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>2</v>
       </c>
@@ -2987,7 +3126,7 @@
         <v>-269.24954985198525</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>1</v>
       </c>
@@ -3007,7 +3146,7 @@
         <v>11.947996459852902</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>2</v>
       </c>
@@ -3027,7 +3166,7 @@
         <v>-35.187841425824786</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -3047,7 +3186,7 @@
         <v>-29.09939878536332</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>0</v>
       </c>
@@ -3067,7 +3206,7 @@
         <v>451.23142185735645</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>1</v>
       </c>
@@ -3087,7 +3226,7 @@
         <v>-86.306344798120108</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>2</v>
       </c>
@@ -3107,7 +3246,7 @@
         <v>-11.673329874568878</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>3</v>
       </c>
@@ -3127,7 +3266,7 @@
         <v>-384.06018250068666</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>0</v>
       </c>
@@ -3147,7 +3286,7 @@
         <v>66.637165440839865</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>1</v>
       </c>
@@ -3167,7 +3306,7 @@
         <v>12.070070497756831</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>2</v>
       </c>
@@ -3187,7 +3326,7 @@
         <v>31.311990722373139</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>3</v>
       </c>
@@ -3207,7 +3346,7 @@
         <v>190.43549913022247</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>0</v>
       </c>
@@ -3227,7 +3366,7 @@
         <v>-128.39136936552023</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>1</v>
       </c>
@@ -3247,7 +3386,7 @@
         <v>146.99240089114048</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>2</v>
       </c>
@@ -3267,7 +3406,7 @@
         <v>-21.134067812128023</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>1</v>
       </c>
@@ -3287,7 +3426,7 @@
         <v>81.484420300912518</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>2</v>
       </c>
@@ -3307,7 +3446,7 @@
         <v>-313.50138859218112</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>3</v>
       </c>
@@ -3327,7 +3466,7 @@
         <v>-240.57741019928585</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>0</v>
       </c>
@@ -3347,7 +3486,7 @@
         <v>-27.207251197851406</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>1</v>
       </c>
@@ -3367,7 +3506,7 @@
         <v>169.80498672444838</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>2</v>
       </c>
@@ -3387,7 +3526,7 @@
         <v>116.97744682149721</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>3</v>
       </c>
@@ -3407,7 +3546,7 @@
         <v>134.31196020386363</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>0</v>
       </c>
@@ -3427,7 +3566,7 @@
         <v>102.61848811304054</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>1</v>
       </c>
@@ -3447,7 +3586,7 @@
         <v>-81.820123905148478</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>2</v>
       </c>
@@ -3467,7 +3606,7 @@
         <v>-88.85464033936583</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>3</v>
       </c>
@@ -3487,7 +3626,7 @@
         <v>6.6835535752433834</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>0</v>
       </c>
@@ -3507,7 +3646,7 @@
         <v>-211.82897427289655</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>1</v>
       </c>
@@ -3527,7 +3666,7 @@
         <v>-207.84630878627888</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>2</v>
       </c>
@@ -3547,7 +3686,7 @@
         <v>351.96996978667562</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>1</v>
       </c>
@@ -3567,7 +3706,7 @@
         <v>218.75667592394788</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>2</v>
       </c>
@@ -3587,7 +3726,7 @@
         <v>291.14658040101324</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>3</v>
       </c>
@@ -3607,7 +3746,7 @@
         <v>200.20142216254158</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>0</v>
       </c>
@@ -3627,7 +3766,7 @@
         <v>122.15033417767876</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>1</v>
       </c>
@@ -3647,7 +3786,7 @@
         <v>115.11581774346143</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>2</v>
       </c>
@@ -3667,7 +3806,7 @@
         <v>-207.12912381359294</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>3</v>
       </c>
@@ -3687,7 +3826,7 @@
         <v>-359.03500473036894</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>0</v>
       </c>
@@ -3707,7 +3846,7 @@
         <v>79.378643147068701</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>1</v>
       </c>
@@ -3727,7 +3866,7 @@
         <v>363.81115146336253</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>2</v>
       </c>
@@ -3747,7 +3886,7 @@
         <v>-23.758659627063821</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>3</v>
       </c>
@@ -3767,7 +3906,7 @@
         <v>245.04837183751948</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -3787,7 +3926,7 @@
         <v>-120.94485305337687</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>1</v>
       </c>
@@ -3807,7 +3946,7 @@
         <v>-109.40885647144994</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>2</v>
       </c>
@@ -3827,7 +3966,7 @@
         <v>48.738059633167509</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>1</v>
       </c>
@@ -3847,7 +3986,7 @@
         <v>-101.35196996978669</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>2</v>
       </c>
@@ -3867,7 +4006,7 @@
         <v>-117.66411328470716</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>3</v>
       </c>
@@ -3887,7 +4026,7 @@
         <v>114.18500320444349</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>0</v>
       </c>
@@ -3907,7 +4046,7 @@
         <v>144.67299417096467</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>1</v>
       </c>
@@ -3927,7 +4066,7 @@
         <v>137.07388531144142</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>2</v>
       </c>
@@ -3947,7 +4086,7 @@
         <v>286.64510025330367</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>3</v>
       </c>
@@ -3967,7 +4106,7 @@
         <v>169.51506088442639</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>0</v>
       </c>
@@ -3987,7 +4126,7 @@
         <v>43.610950041200056</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>1</v>
       </c>
@@ -4007,7 +4146,7 @@
         <v>-5.0965910824914999</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>2</v>
       </c>
@@ -4027,7 +4166,7 @@
         <v>-83.498641926328318</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>3</v>
       </c>
@@ -4047,7 +4186,7 @@
         <v>306.93990905484179</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>0</v>
       </c>
@@ -4067,7 +4206,7 @@
         <v>142.8113650929289</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>1</v>
       </c>
@@ -4087,7 +4226,7 @@
         <v>0.97659230323193924</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -4107,7 +4246,7 @@
         <v>-388.0581072420423</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>1</v>
       </c>
@@ -4127,7 +4266,7 @@
         <v>154.6983245338298</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>2</v>
       </c>
@@ -4147,7 +4286,7 @@
         <v>-378.97885067293311</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>3</v>
       </c>
@@ -4167,7 +4306,7 @@
         <v>5.2186651203954852</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>0</v>
       </c>
@@ -4187,7 +4326,7 @@
         <v>152.18054750205999</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>1</v>
       </c>
@@ -4207,7 +4346,7 @@
         <v>32.197027497177039</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -4227,7 +4366,7 @@
         <v>231.33030182805871</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>3</v>
       </c>
@@ -4247,7 +4386,7 @@
         <v>25.116733298745686</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>0</v>
       </c>
@@ -4267,7 +4406,7 @@
         <v>-348.38404492324594</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>1</v>
       </c>
@@ -4287,7 +4426,7 @@
         <v>1.4038514358958309</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>2</v>
       </c>
@@ -4307,7 +4446,7 @@
         <v>160.00854518265328</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>3</v>
       </c>
@@ -4327,7 +4466,7 @@
         <v>-200.79653309732353</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>0</v>
       </c>
@@ -4347,7 +4486,7 @@
         <v>-133.44218268379777</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>1</v>
       </c>
@@ -4367,7 +4506,7 @@
         <v>-155.73595385601368</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>2</v>
       </c>
@@ -4387,7 +4526,7 @@
         <v>-110.12604144413589</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>1</v>
       </c>
@@ -4407,7 +4546,7 @@
         <v>235.0383007293924</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>2</v>
       </c>
@@ -4427,7 +4566,7 @@
         <v>349.00967436750392</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>3</v>
       </c>
@@ -4447,7 +4586,7 @@
         <v>-346.81234168523213</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>0</v>
       </c>
@@ -4467,7 +4606,7 @@
         <v>4.5319986571855679</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>1</v>
       </c>
@@ -4487,7 +4626,7 @@
         <v>-60.838648640400422</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>2</v>
       </c>
@@ -4507,7 +4646,7 @@
         <v>-114.03241065706345</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>3</v>
       </c>
@@ -4527,7 +4666,7 @@
         <v>222.47993408001952</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>0</v>
       </c>
@@ -4547,7 +4686,7 @@
         <v>-128.19299905392617</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>1</v>
       </c>
@@ -4567,7 +4706,7 @@
         <v>16.846217230750426</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>2</v>
       </c>
@@ -4587,7 +4726,7 @@
         <v>161.35135959959717</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>3</v>
       </c>
@@ -4607,7 +4746,7 @@
         <v>-72.099978637043364</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>0</v>
       </c>
@@ -4627,7 +4766,7 @@
         <v>-356.54774620807518</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>1</v>
       </c>
@@ -4647,7 +4786,7 @@
         <v>-171.5598010193182</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>2</v>
       </c>
@@ -4667,7 +4806,7 @@
         <v>77.944273201696831</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>1</v>
       </c>
@@ -4687,7 +4826,7 @@
         <v>282.15887936033209</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>2</v>
       </c>
@@ -4707,7 +4846,7 @@
         <v>8.8656270027771882</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>3</v>
       </c>
@@ -4727,7 +4866,7 @@
         <v>-109.27152317880791</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>0</v>
       </c>
@@ -4747,7 +4886,7 @@
         <v>-322.94686727500226</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>1</v>
       </c>
@@ -4767,7 +4906,7 @@
         <v>353.55693227942749</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>2</v>
       </c>
@@ -4787,7 +4926,7 @@
         <v>140.07995849482708</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>3</v>
       </c>
@@ -4807,7 +4946,7 @@
         <v>109.89715262306589</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>0</v>
       </c>
@@ -4827,7 +4966,7 @@
         <v>93.46293527024136</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>1</v>
       </c>
@@ -4847,7 +4986,7 @@
         <v>-264.50392162846765</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>2</v>
       </c>
@@ -4867,7 +5006,7 @@
         <v>-234.21430097354045</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>3</v>
       </c>
@@ -4887,7 +5026,7 @@
         <v>34.318063905758841</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>0</v>
       </c>
@@ -4907,7 +5046,7 @@
         <v>-17.22769859920038</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>1</v>
       </c>
@@ -4927,7 +5066,7 @@
         <v>254.34125797296056</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>2</v>
       </c>
@@ -4947,7 +5086,7 @@
         <v>-188.19238868373668</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>1</v>
       </c>
@@ -4967,7 +5106,7 @@
         <v>314.27961058381908</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>2</v>
       </c>
@@ -4987,7 +5126,7 @@
         <v>-140.84292123172702</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>3</v>
       </c>
@@ -5007,7 +5146,7 @@
         <v>102.67952513199253</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>0</v>
       </c>
@@ -5027,7 +5166,7 @@
         <v>45.152134769737842</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>1</v>
       </c>
@@ -5047,7 +5186,7 @@
         <v>56.169316690572828</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>2</v>
       </c>
@@ -5067,7 +5206,7 @@
         <v>-219.35178685872981</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>3</v>
       </c>
@@ -5087,7 +5226,7 @@
         <v>86.504715109714056</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>0</v>
       </c>
@@ -5107,7 +5246,7 @@
         <v>159.93224890896329</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>1</v>
       </c>
@@ -5127,7 +5266,7 @@
         <v>258.78170110171811</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>2</v>
       </c>
@@ -5147,7 +5286,7 @@
         <v>319.51353495895262</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>3</v>
       </c>
@@ -5167,7 +5306,7 @@
         <v>-327.44834742271183</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>0</v>
       </c>
@@ -5187,7 +5326,7 @@
         <v>-258.17133091219819</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>1</v>
       </c>
@@ -5207,7 +5346,7 @@
         <v>19.135105441450207</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>2</v>
       </c>
@@ -5227,7 +5366,7 @@
         <v>-244.54481643116554</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>1</v>
       </c>
@@ -5247,7 +5386,7 @@
         <v>24.353770561845749</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>2</v>
       </c>
@@ -5267,7 +5406,7 @@
         <v>49.226355784783436</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>3</v>
       </c>
@@ -5287,7 +5426,7 @@
         <v>195.34897915585807</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>0</v>
       </c>
@@ -5307,7 +5446,7 @@
         <v>-71.077608569597473</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>1</v>
       </c>
@@ -5327,7 +5466,7 @@
         <v>213.78215887936034</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>2</v>
       </c>
@@ -5347,7 +5486,7 @@
         <v>47.959837641529617</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>3</v>
       </c>
@@ -5367,7 +5506,7 @@
         <v>213.91949217200238</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>0</v>
       </c>
@@ -5387,7 +5526,7 @@
         <v>-308.0996124149296</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>1</v>
       </c>
@@ -5407,7 +5546,7 @@
         <v>-203.8941618091373</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>2</v>
       </c>
@@ -5427,7 +5566,7 @@
         <v>137.76055177465139</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>3</v>
       </c>
@@ -5447,7 +5586,7 @@
         <v>209.21964171269877</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>0</v>
       </c>
@@ -5467,7 +5606,7 @@
         <v>-105.89922788171026</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>1</v>
       </c>
@@ -5487,7 +5626,7 @@
         <v>-64.34827723014007</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>2</v>
       </c>
@@ -5507,7 +5646,7 @@
         <v>7.385479293191338</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>1</v>
       </c>
@@ -5527,7 +5666,7 @@
         <v>-317.60612811670279</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>2</v>
       </c>
@@ -5547,7 +5686,7 @@
         <v>-158.34528641621145</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>3</v>
       </c>
@@ -5567,7 +5706,7 @@
         <v>269.89043855098112</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>0</v>
       </c>
@@ -5587,7 +5726,7 @@
         <v>56.382946256904816</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>1</v>
       </c>
@@ -5607,7 +5746,7 @@
         <v>-132.6792199468978</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>2</v>
       </c>
@@ -5627,7 +5766,7 @@
         <v>-333.93353068636128</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>3</v>
       </c>
@@ -5647,7 +5786,7 @@
         <v>199.11801507614365</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>0</v>
       </c>
@@ -5667,7 +5806,7 @@
         <v>-179.5251319925535</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>1</v>
       </c>
@@ -5687,7 +5826,7 @@
         <v>-8.8656270027772166</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>2</v>
       </c>
@@ -5707,7 +5846,7 @@
         <v>40.681173131504238</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>3</v>
       </c>
@@ -5727,7 +5866,7 @@
         <v>-210.36408581804861</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>0</v>
       </c>
@@ -5747,7 +5886,7 @@
         <v>-161.38187810907317</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>1</v>
       </c>
@@ -5767,7 +5906,7 @@
         <v>116.71803949095124</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>2</v>
       </c>
@@ -5787,7 +5926,7 @@
         <v>182.45490890224926</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>1</v>
       </c>
@@ -5807,7 +5946,7 @@
         <v>-22.38532670064393</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>2</v>
       </c>
@@ -5827,7 +5966,7 @@
         <v>-101.19937742240671</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>3</v>
       </c>
@@ -5847,7 +5986,7 @@
         <v>-245.2314828943754</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>0</v>
       </c>
@@ -5867,7 +6006,7 @@
         <v>76.281014435254974</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>1</v>
       </c>
@@ -5887,7 +6026,7 @@
         <v>-238.88363292336803</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A274" t="s">
         <v>2</v>
       </c>
@@ -5907,7 +6046,7 @@
         <v>100.26856288338877</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>3</v>
       </c>
@@ -5927,7 +6066,7 @@
         <v>-67.049165318765859</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A276" t="s">
         <v>0</v>
       </c>
@@ -5947,7 +6086,7 @@
         <v>-140.4004028443251</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A277" t="s">
         <v>1</v>
       </c>
@@ -5967,7 +6106,7 @@
         <v>68.132572405163728</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A278" t="s">
         <v>2</v>
       </c>
@@ -5987,7 +6126,7 @@
         <v>-330.24079103976561</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
         <v>3</v>
       </c>
@@ -6007,7 +6146,7 @@
         <v>-90.517899105807629</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
         <v>0</v>
       </c>
@@ -6027,7 +6166,7 @@
         <v>-195.56260872218999</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
         <v>1</v>
       </c>
@@ -6047,7 +6186,7 @@
         <v>-12.283700064088805</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
         <v>2</v>
       </c>
@@ -6067,7 +6206,7 @@
         <v>-30.94576860866114</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A283" t="s">
         <v>1</v>
       </c>
@@ -6087,7 +6226,7 @@
         <v>218.72615741447191</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A284" t="s">
         <v>2</v>
       </c>
@@ -6107,7 +6246,7 @@
         <v>334.87960448011722</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A285" t="s">
         <v>3</v>
       </c>
@@ -6127,7 +6266,7 @@
         <v>52.03405865657524</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
         <v>0</v>
       </c>
@@ -6147,7 +6286,7 @@
         <v>-368.66359447004612</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>1</v>
       </c>
@@ -6167,7 +6306,7 @@
         <v>236.45741142002623</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
         <v>2</v>
       </c>
@@ -6187,7 +6326,7 @@
         <v>16.891994994964477</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>3</v>
       </c>
@@ -6207,7 +6346,7 @@
         <v>-243.46140934476762</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>0</v>
       </c>
@@ -6227,7 +6366,7 @@
         <v>264.35132908108773</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>1</v>
       </c>
@@ -6247,7 +6386,7 @@
         <v>-47.990356151005585</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
         <v>2</v>
       </c>
@@ -6267,7 +6406,7 @@
         <v>-41.322061830500161</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>3</v>
       </c>
@@ -6287,7 +6426,7 @@
         <v>6.0884426404614373</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A294" t="s">
         <v>0</v>
       </c>
@@ -6307,7 +6446,7 @@
         <v>156.80410168767355</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>1</v>
       </c>
@@ -6327,7 +6466,7 @@
         <v>-364.83352153080847</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>2</v>
       </c>
@@ -6347,7 +6486,7 @@
         <v>-441.67912839136937</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>1</v>
       </c>
@@ -6367,7 +6506,7 @@
         <v>-325.78508865627003</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A298" t="s">
         <v>2</v>
       </c>
@@ -6387,7 +6526,7 @@
         <v>-73.122348704489241</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>3</v>
       </c>
@@ -6407,7 +6546,7 @@
         <v>84.780419324320235</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
         <v>0</v>
       </c>
@@ -6427,7 +6566,7 @@
         <v>36.820581682790618</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>1</v>
       </c>
@@ -6447,7 +6586,7 @@
         <v>-36.683248390148663</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
         <v>2</v>
       </c>
@@ -6467,7 +6606,7 @@
         <v>49.226355784783436</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>3</v>
       </c>
@@ -6487,7 +6626,7 @@
         <v>147.11447492904446</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A304" t="s">
         <v>0</v>
       </c>
@@ -6507,7 +6646,7 @@
         <v>-306.34479812005981</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
         <v>1</v>
       </c>
@@ -6527,7 +6666,7 @@
         <v>-247.07785271767324</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
         <v>2</v>
       </c>
@@ -6547,7 +6686,7 @@
         <v>-301.56865138706621</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
         <v>3</v>
       </c>
@@ -6567,7 +6706,7 @@
         <v>191.2594988860744</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A308" t="s">
         <v>0</v>
       </c>
@@ -6587,7 +6726,7 @@
         <v>-177.40409558397164</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
         <v>1</v>
       </c>
@@ -6607,7 +6746,7 @@
         <v>-376.00329599902341</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A310" t="s">
         <v>2</v>
       </c>
@@ -6627,7 +6766,7 @@
         <v>-153.55388042847986</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A311" t="s">
         <v>1</v>
       </c>
@@ -6647,7 +6786,7 @@
         <v>228.93459883419294</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
         <v>2</v>
       </c>
@@ -6667,7 +6806,7 @@
         <v>-274.88021485030674</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
         <v>3</v>
       </c>
@@ -6687,7 +6826,7 @@
         <v>246.29963072603533</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
         <v>0</v>
       </c>
@@ -6707,7 +6846,7 @@
         <v>51.438947721793227</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
         <v>1</v>
       </c>
@@ -6727,7 +6866,7 @@
         <v>366.43574327829828</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A316" t="s">
         <v>2</v>
       </c>
@@ -6747,7 +6886,7 @@
         <v>258.9953306680502</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A317" t="s">
         <v>3</v>
       </c>
@@ -6767,7 +6906,7 @@
         <v>316.61427655873285</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A318" t="s">
         <v>0</v>
       </c>
@@ -6787,7 +6926,7 @@
         <v>-124.50025940733053</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
         <v>1</v>
       </c>
@@ -6807,7 +6946,7 @@
         <v>276.0399182103946</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A320" t="s">
         <v>2</v>
       </c>
@@ -6827,7 +6966,7 @@
         <v>-140.52247688222909</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A321" t="s">
         <v>3</v>
       </c>
@@ -6847,7 +6986,7 @@
         <v>-264.68703268532363</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A322" t="s">
         <v>0</v>
       </c>
@@ -6867,7 +7006,7 @@
         <v>-131.21433149204992</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A323" t="s">
         <v>1</v>
       </c>
@@ -6887,7 +7026,7 @@
         <v>374.49262977996159</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A324" t="s">
         <v>2</v>
       </c>
@@ -6907,7 +7046,7 @@
         <v>-29.145176549577343</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A325" t="s">
         <v>1</v>
       </c>
@@ -6927,7 +7066,7 @@
         <v>208.68556779686881</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A326" t="s">
         <v>2</v>
       </c>
@@ -6947,7 +7086,7 @@
         <v>57.512131107516723</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>3</v>
       </c>
@@ -6967,7 +7106,7 @@
         <v>-104.00708029419842</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A328" t="s">
         <v>0</v>
       </c>
@@ -6987,7 +7126,7 @@
         <v>325.28153324991609</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A329" t="s">
         <v>1</v>
       </c>
@@ -7007,7 +7146,7 @@
         <v>-35.630359813226718</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A330" t="s">
         <v>2</v>
       </c>
@@ -7027,7 +7166,7 @@
         <v>-126.59077730643631</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A331" t="s">
         <v>3</v>
       </c>
@@ -7047,7 +7186,7 @@
         <v>47.242652668843675</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A332" t="s">
         <v>0</v>
       </c>
@@ -7067,7 +7206,7 @@
         <v>7.1413312173833106</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A333" t="s">
         <v>1</v>
       </c>
@@ -7087,7 +7226,7 @@
         <v>-232.15430158391067</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A334" t="s">
         <v>2</v>
       </c>
@@ -7107,7 +7246,7 @@
         <v>-37.81243324076047</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A335" t="s">
         <v>3</v>
       </c>
@@ -7127,7 +7266,7 @@
         <v>-68.025757621997741</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A336" t="s">
         <v>0</v>
       </c>
@@ -7147,7 +7286,7 @@
         <v>239.90600299081393</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A337" t="s">
         <v>1</v>
       </c>
@@ -7167,7 +7306,7 @@
         <v>427.06076235236668</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A338" t="s">
         <v>2</v>
       </c>
@@ -7187,7 +7326,7 @@
         <v>-191.93090609454632</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A339" t="s">
         <v>1</v>
       </c>
@@ -7207,7 +7346,7 @@
         <v>-67.415387432477786</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A340" t="s">
         <v>2</v>
       </c>
@@ -7227,7 +7366,7 @@
         <v>-166.95150608844267</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A341" t="s">
         <v>3</v>
       </c>
@@ -7247,7 +7386,7 @@
         <v>-27.283547471541489</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A342" t="s">
         <v>0</v>
       </c>
@@ -7267,7 +7406,7 @@
         <v>112.67433698538161</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>1</v>
       </c>
@@ -7287,7 +7426,7 @@
         <v>236.19800408948026</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
         <v>2</v>
       </c>
@@ -7307,7 +7446,7 @@
         <v>226.8898586993011</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>3</v>
       </c>
@@ -7327,7 +7466,7 @@
         <v>202.18512527848142</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A346" t="s">
         <v>0</v>
       </c>
@@ -7347,7 +7486,7 @@
         <v>-135.0901821955016</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A347" t="s">
         <v>1</v>
       </c>
@@ -7367,7 +7506,7 @@
         <v>-307.15353862117377</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A348" t="s">
         <v>2</v>
       </c>
@@ -7387,7 +7526,7 @@
         <v>72.252571184423402</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
         <v>3</v>
       </c>
@@ -7407,7 +7546,7 @@
         <v>-226.21845149082918</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>0</v>
       </c>
@@ -7427,7 +7566,7 @@
         <v>-459.8681600390637</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>1</v>
       </c>
@@ -7447,7 +7586,7 @@
         <v>193.27372051149021</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A352" t="s">
         <v>2</v>
       </c>
@@ -7467,7 +7606,7 @@
         <v>283.07443464461193</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A353" t="s">
         <v>1</v>
       </c>
@@ -7487,7 +7626,7 @@
         <v>39.719840083010297</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A354" t="s">
         <v>2</v>
       </c>
@@ -7507,7 +7646,7 @@
         <v>-134.67818231757559</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A355" t="s">
         <v>3</v>
       </c>
@@ -7527,7 +7666,7 @@
         <v>253.4104434339427</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A356" t="s">
         <v>0</v>
       </c>
@@ -7547,7 +7686,7 @@
         <v>-1.0071108127078787</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
         <v>1</v>
       </c>
@@ -7567,7 +7706,7 @@
         <v>-195.54734946745199</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A358" t="s">
         <v>2</v>
       </c>
@@ -7587,7 +7726,7 @@
         <v>88.534195989867854</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A359" t="s">
         <v>3</v>
       </c>
@@ -7607,7 +7746,7 @@
         <v>-6.1799981688894263</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A360" t="s">
         <v>0</v>
       </c>
@@ -7627,7 +7766,7 @@
         <v>395.7487716299936</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
         <v>1</v>
       </c>
@@ -7647,7 +7786,7 @@
         <v>196.72231208227794</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A362" t="s">
         <v>2</v>
       </c>
@@ -7667,7 +7806,7 @@
         <v>-310.54109317300947</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A363" t="s">
         <v>3</v>
       </c>
@@ -7687,7 +7826,7 @@
         <v>200.90334788048949</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A364" t="s">
         <v>0</v>
       </c>
@@ -7707,7 +7846,7 @@
         <v>280.41932432020019</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A365" t="s">
         <v>1</v>
       </c>
@@ -7727,7 +7866,7 @@
         <v>-158.08587908566543</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A366" t="s">
         <v>2</v>
       </c>
@@ -7747,7 +7886,7 @@
         <v>-30.808435316019143</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A367" t="s">
         <v>1</v>
       </c>
@@ -7767,7 +7906,7 @@
         <v>157.7349162266915</v>
       </c>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A368" t="s">
         <v>2</v>
       </c>
@@ -7787,7 +7926,7 @@
         <v>-90.166936246833728</v>
       </c>
     </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A369" t="s">
         <v>3</v>
       </c>
@@ -7807,7 +7946,7 @@
         <v>23.209326456495866</v>
       </c>
     </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A370" t="s">
         <v>0</v>
       </c>
@@ -7827,7 +7966,7 @@
         <v>-43.961912900173957</v>
       </c>
     </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A371" t="s">
         <v>1</v>
       </c>
@@ -7847,7 +7986,7 @@
         <v>-68.132572405163785</v>
       </c>
     </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A372" t="s">
         <v>2</v>
       </c>
@@ -7867,7 +8006,7 @@
         <v>-31.388286996063101</v>
       </c>
     </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A373" t="s">
         <v>3</v>
       </c>
@@ -7887,7 +8026,7 @@
         <v>18.066957609790336</v>
       </c>
     </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A374" t="s">
         <v>0</v>
       </c>
@@ -7907,7 +8046,7 @@
         <v>65.599536118655948</v>
       </c>
     </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A375" t="s">
         <v>1</v>
       </c>
@@ -7927,7 +8066,7 @@
         <v>-192.28186895352033</v>
       </c>
     </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A376" t="s">
         <v>2</v>
       </c>
@@ -7947,7 +8086,7 @@
         <v>-354.80819116794333</v>
       </c>
     </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A377" t="s">
         <v>3</v>
       </c>
@@ -7967,7 +8106,7 @@
         <v>298.25739310892055</v>
       </c>
     </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A378" t="s">
         <v>0</v>
       </c>
@@ -7987,7 +8126,7 @@
         <v>-48.036133915219636</v>
       </c>
     </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A379" t="s">
         <v>1</v>
       </c>
@@ -8007,7 +8146,7 @@
         <v>-448.97305215613267</v>
       </c>
     </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A380" t="s">
         <v>2</v>
       </c>
@@ -8027,7 +8166,7 @@
         <v>242.91207617419965</v>
       </c>
     </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A381" t="s">
         <v>1</v>
       </c>
@@ -8047,7 +8186,7 @@
         <v>-219.47386089663379</v>
       </c>
     </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A382" t="s">
         <v>2</v>
       </c>
@@ -8067,7 +8206,7 @@
         <v>-11.963255714590929</v>
       </c>
     </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A383" t="s">
         <v>3</v>
       </c>
@@ -8087,7 +8226,7 @@
         <v>192.75490585039825</v>
       </c>
     </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A384" t="s">
         <v>0</v>
       </c>
@@ -8107,7 +8246,7 @@
         <v>-236.33533738212222</v>
       </c>
     </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A385" t="s">
         <v>1</v>
       </c>
@@ -8127,7 +8266,7 @@
         <v>315.71398052919096</v>
       </c>
     </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A386" t="s">
         <v>2</v>
       </c>
@@ -8147,7 +8286,7 @@
         <v>-187.93298135319071</v>
       </c>
     </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A387" t="s">
         <v>3</v>
       </c>
@@ -8167,7 +8306,7 @@
         <v>19.898068178350172</v>
       </c>
     </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A388" t="s">
         <v>0</v>
       </c>
@@ -8187,7 +8326,7 @@
         <v>-98.025452436902981</v>
       </c>
     </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A389" t="s">
         <v>1</v>
       </c>
@@ -8207,7 +8346,7 @@
         <v>103.47300637836848</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A390" t="s">
         <v>2</v>
       </c>
@@ -8227,7 +8366,7 @@
         <v>378.29218420972319</v>
       </c>
     </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A391" t="s">
         <v>3</v>
       </c>
@@ -8247,7 +8386,7 @@
         <v>-38.666951506088452</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A392" t="s">
         <v>0</v>
       </c>
@@ -8267,7 +8406,7 @@
         <v>-113.63567003387556</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A393" t="s">
         <v>1</v>
       </c>
@@ -8287,7 +8426,7 @@
         <v>-279.64110232856223</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A394" t="s">
         <v>2</v>
       </c>
@@ -8307,7 +8446,7 @@
         <v>448.77468184453869</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A395" t="s">
         <v>1</v>
       </c>
@@ -8327,7 +8466,7 @@
         <v>55.00961333048491</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A396" t="s">
         <v>2</v>
       </c>
@@ -8347,7 +8486,7 @@
         <v>-393.87188329721977</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A397" t="s">
         <v>3</v>
       </c>
@@ -8367,7 +8506,7 @@
         <v>-51.332132938627296</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A398" t="s">
         <v>0</v>
       </c>
@@ -8387,7 +8526,7 @@
         <v>-35.706656086916666</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A399" t="s">
         <v>1</v>
       </c>
@@ -8407,7 +8546,7 @@
         <v>185.20157475508896</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A400" t="s">
         <v>2</v>
       </c>
@@ -8427,7 +8566,7 @@
         <v>-39.231543931394356</v>
       </c>
     </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A401" t="s">
         <v>3</v>
       </c>
@@ -8447,7 +8586,7 @@
         <v>-406.33869441816461</v>
       </c>
     </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A402" t="s">
         <v>0</v>
       </c>
@@ -8467,7 +8606,7 @@
         <v>231.71178319650872</v>
       </c>
     </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A403" t="s">
         <v>1</v>
       </c>
@@ -8487,7 +8626,7 @@
         <v>276.5129551072726</v>
       </c>
     </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A404" t="s">
         <v>2</v>
       </c>
@@ -8507,7 +8646,7 @@
         <v>369.39603869747003</v>
       </c>
     </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A405" t="s">
         <v>3</v>
       </c>
@@ -8527,7 +8666,7 @@
         <v>-23.621326334421838</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A406" t="s">
         <v>0</v>
       </c>
@@ -8547,7 +8686,7 @@
         <v>-135.09018219550154</v>
       </c>
     </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A407" t="s">
         <v>1</v>
       </c>
@@ -8567,7 +8706,7 @@
         <v>132.54188665425582</v>
       </c>
     </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A408" t="s">
         <v>2</v>
       </c>
@@ -8587,7 +8726,7 @@
         <v>-122.0130008850368</v>
       </c>
     </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A409" t="s">
         <v>1</v>
       </c>
@@ -8607,7 +8746,7 @@
         <v>289.88006225775933</v>
       </c>
     </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A410" t="s">
         <v>2</v>
       </c>
@@ -8627,7 +8766,7 @@
         <v>-82.430494094668404</v>
       </c>
     </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A411" t="s">
         <v>3</v>
       </c>
@@ -8647,7 +8786,7 @@
         <v>106.54011658070618</v>
       </c>
     </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A412" t="s">
         <v>0</v>
       </c>
@@ -8667,7 +8806,7 @@
         <v>-198.29401532029175</v>
       </c>
     </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A413" t="s">
         <v>1</v>
       </c>
@@ -8687,7 +8826,7 @@
         <v>6.241035187841419</v>
       </c>
     </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A414" t="s">
         <v>2</v>
       </c>
@@ -8707,7 +8846,7 @@
         <v>144.50514236884669</v>
       </c>
     </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A415" t="s">
         <v>3</v>
       </c>
@@ -8727,7 +8866,7 @@
         <v>-208.47193823053681</v>
       </c>
     </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A416" t="s">
         <v>0</v>
       </c>
@@ -8747,7 +8886,7 @@
         <v>-160.10010071108127</v>
       </c>
     </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A417" t="s">
         <v>1</v>
       </c>
@@ -8767,7 +8906,7 @@
         <v>21.805475020599999</v>
       </c>
     </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A418" t="s">
         <v>2</v>
       </c>
@@ -8787,7 +8926,7 @@
         <v>-170.38483840449231</v>
       </c>
     </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A419" t="s">
         <v>3</v>
       </c>
@@ -8807,7 +8946,7 @@
         <v>-82.354197820978413</v>
       </c>
     </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A420" t="s">
         <v>0</v>
       </c>
@@ -8827,7 +8966,7 @@
         <v>-398.78536332285529</v>
       </c>
     </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A421" t="s">
         <v>1</v>
       </c>
@@ -8847,7 +8986,7 @@
         <v>228.27845088045899</v>
       </c>
     </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A422" t="s">
         <v>2</v>
       </c>
@@ -8867,7 +9006,7 @@
         <v>117.69463179418318</v>
       </c>
     </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A423" t="s">
         <v>1</v>
       </c>
@@ -8887,7 +9026,7 @@
         <v>143.78795739616078</v>
       </c>
     </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A424" t="s">
         <v>2</v>
       </c>
@@ -8907,7 +9046,7 @@
         <v>-23.590807824945841</v>
       </c>
     </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A425" t="s">
         <v>3</v>
       </c>
@@ -8927,7 +9066,7 @@
         <v>-303.07931760612814</v>
       </c>
     </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A426" t="s">
         <v>0</v>
       </c>
@@ -8947,7 +9086,7 @@
         <v>287.51487777336956</v>
       </c>
     </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A427" t="s">
         <v>1</v>
       </c>
@@ -8967,7 +9106,7 @@
         <v>431.37913144322033</v>
       </c>
     </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A428" t="s">
         <v>2</v>
       </c>
@@ -8987,7 +9126,7 @@
         <v>-203.65001373332927</v>
       </c>
     </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A429" t="s">
         <v>3</v>
       </c>
@@ -9007,7 +9146,7 @@
         <v>-336.17664113284707</v>
       </c>
     </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A430" t="s">
         <v>0</v>
       </c>
@@ -9027,7 +9166,7 @@
         <v>-95.95019379253516</v>
       </c>
     </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A431" t="s">
         <v>1</v>
       </c>
@@ -9047,7 +9186,7 @@
         <v>187.71935178685874</v>
       </c>
     </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A432" t="s">
         <v>2</v>
       </c>
@@ -9067,7 +9206,7 @@
         <v>-287.45384075441757</v>
       </c>
     </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A433" t="s">
         <v>3</v>
       </c>
@@ -9087,7 +9226,7 @@
         <v>3.1739249855036746</v>
       </c>
     </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A434" t="s">
         <v>0</v>
       </c>
@@ -9107,7 +9246,7 @@
         <v>-213.09549241615036</v>
       </c>
     </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A435" t="s">
         <v>1</v>
       </c>
@@ -9127,7 +9266,7 @@
         <v>366.42048402356028</v>
       </c>
     </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A436" t="s">
         <v>2</v>
       </c>
@@ -9147,7 +9286,7 @@
         <v>-261.97088534195996</v>
       </c>
     </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A437" t="s">
         <v>1</v>
       </c>
@@ -9167,7 +9306,7 @@
         <v>-123.55418561357462</v>
       </c>
     </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A438" t="s">
         <v>2</v>
       </c>
@@ -9187,7 +9326,7 @@
         <v>-267.25058748130743</v>
       </c>
     </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A439" t="s">
         <v>3</v>
       </c>
@@ -9207,7 +9346,7 @@
         <v>212.05786309396649</v>
       </c>
     </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A440" t="s">
         <v>0</v>
       </c>
@@ -9227,7 +9366,7 @@
         <v>-114.29181798760948</v>
       </c>
     </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A441" t="s">
         <v>1</v>
       </c>
@@ -9247,7 +9386,7 @@
         <v>-255.08896145512256</v>
       </c>
     </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A442" t="s">
         <v>2</v>
       </c>
@@ -9267,7 +9406,7 @@
         <v>-70.818201239051518</v>
       </c>
     </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A443" t="s">
         <v>3</v>
       </c>
@@ -9287,7 +9426,7 @@
         <v>337.32108523819699</v>
       </c>
     </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A444" t="s">
         <v>0</v>
       </c>
@@ -9307,7 +9446,7 @@
         <v>341.95989867854854</v>
       </c>
     </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A445" t="s">
         <v>1</v>
       </c>
@@ -9327,7 +9466,7 @@
         <v>-67.140720847193819</v>
       </c>
     </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A446" t="s">
         <v>2</v>
       </c>
@@ -9347,7 +9486,7 @@
         <v>-2.7008880886257529</v>
       </c>
     </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A447" t="s">
         <v>3</v>
       </c>
@@ -9367,7 +9506,7 @@
         <v>319.25412762840665</v>
       </c>
     </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A448" t="s">
         <v>0</v>
       </c>
@@ -9387,7 +9526,7 @@
         <v>112.82692953276161</v>
       </c>
     </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A449" t="s">
         <v>1</v>
       </c>
@@ -9407,7 +9546,7 @@
         <v>-70.98605304116947</v>
       </c>
     </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A450" t="s">
         <v>2</v>
       </c>
@@ -9427,7 +9566,7 @@
         <v>101.07730338450267</v>
       </c>
     </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A451" t="s">
         <v>1</v>
       </c>
@@ -9447,7 +9586,7 @@
         <v>2.8077028717917472</v>
       </c>
     </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A452" t="s">
         <v>2</v>
       </c>
@@ -9467,7 +9606,7 @@
         <v>-419.44639423810543</v>
       </c>
     </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A453" t="s">
         <v>3</v>
       </c>
@@ -9487,7 +9626,7 @@
         <v>113.94085512863552</v>
       </c>
     </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A454" t="s">
         <v>0</v>
       </c>
@@ -9507,7 +9646,7 @@
         <v>60.16724143192846</v>
       </c>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A455" t="s">
         <v>1</v>
       </c>
@@ -9527,7 +9666,7 @@
         <v>198.88912625507371</v>
       </c>
     </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A456" t="s">
         <v>2</v>
       </c>
@@ -9547,7 +9686,7 @@
         <v>-92.440565202795483</v>
       </c>
     </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A457" t="s">
         <v>3</v>
       </c>
@@ -9567,7 +9706,7 @@
         <v>100.57374797814873</v>
       </c>
     </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A458" t="s">
         <v>0</v>
       </c>
@@ -9587,7 +9726,7 @@
         <v>404.49232459486677</v>
       </c>
     </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A459" t="s">
         <v>1</v>
       </c>
@@ -9607,7 +9746,7 @@
         <v>-35.782952360606657</v>
       </c>
     </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A460" t="s">
         <v>2</v>
       </c>
@@ -9627,7 +9766,7 @@
         <v>225.54704428235726</v>
       </c>
     </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A461" t="s">
         <v>3</v>
       </c>
@@ -9647,7 +9786,7 @@
         <v>-124.45448164311654</v>
       </c>
     </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A462" t="s">
         <v>0</v>
       </c>
@@ -9667,7 +9806,7 @@
         <v>-192.51075777459027</v>
       </c>
     </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A463" t="s">
         <v>1</v>
       </c>
@@ -9687,7 +9826,7 @@
         <v>-348.87234107486194</v>
       </c>
     </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A464" t="s">
         <v>2</v>
       </c>
@@ -9707,7 +9846,7 @@
         <v>47.502059999389587</v>
       </c>
     </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A465" t="s">
         <v>1</v>
       </c>
@@ -9727,7 +9866,7 @@
         <v>-71.047090060121448</v>
       </c>
     </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A466" t="s">
         <v>2</v>
       </c>
@@ -9747,7 +9886,7 @@
         <v>336.02404858546709</v>
       </c>
     </row>
-    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A467" t="s">
         <v>3</v>
       </c>
@@ -9767,7 +9906,7 @@
         <v>-86.046937467574082</v>
       </c>
     </row>
-    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A468" t="s">
         <v>0</v>
       </c>
@@ -9787,7 +9926,7 @@
         <v>-160.29847102267524</v>
       </c>
     </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A469" t="s">
         <v>1</v>
       </c>
@@ -9807,7 +9946,7 @@
         <v>59.602649006622528</v>
       </c>
     </row>
-    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A470" t="s">
         <v>2</v>
       </c>
@@ -9827,7 +9966,7 @@
         <v>-46.174504837183775</v>
       </c>
     </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A471" t="s">
         <v>3</v>
       </c>
@@ -9847,7 +9986,7 @@
         <v>-139.74425489059115</v>
       </c>
     </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A472" t="s">
         <v>0</v>
       </c>
@@ -9867,7 +10006,7 @@
         <v>-308.67946409497358</v>
       </c>
     </row>
-    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A473" t="s">
         <v>1</v>
       </c>
@@ -9887,7 +10026,7 @@
         <v>43.778801843317979</v>
       </c>
     </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A474" t="s">
         <v>2</v>
       </c>
@@ -9907,7 +10046,7 @@
         <v>216.80349131748409</v>
       </c>
     </row>
-    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A475" t="s">
         <v>3</v>
       </c>
@@ -9927,7 +10066,7 @@
         <v>33.936582537308823</v>
       </c>
     </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A476" t="s">
         <v>0</v>
       </c>
@@ -9947,7 +10086,7 @@
         <v>19.363994262520237</v>
       </c>
     </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A477" t="s">
         <v>1</v>
       </c>
@@ -9967,7 +10106,7 @@
         <v>-145.14603106784261</v>
       </c>
     </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A478" t="s">
         <v>2</v>
       </c>
@@ -9987,7 +10126,7 @@
         <v>96.774193548387103</v>
       </c>
     </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A479" t="s">
         <v>1</v>
       </c>
@@ -10007,7 +10146,7 @@
         <v>-82.049012726218436</v>
       </c>
     </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A480" t="s">
         <v>2</v>
       </c>
@@ -10027,7 +10166,7 @@
         <v>246.00970488601337</v>
       </c>
     </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A481" t="s">
         <v>3</v>
       </c>
@@ -10047,7 +10186,7 @@
         <v>120.82277901547289</v>
       </c>
     </row>
-    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A482" t="s">
         <v>0</v>
       </c>
@@ -10067,7 +10206,7 @@
         <v>-127.94885097811823</v>
       </c>
     </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A483" t="s">
         <v>1</v>
       </c>
@@ -10087,7 +10226,7 @@
         <v>144.01684621723069</v>
       </c>
     </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A484" t="s">
         <v>2</v>
       </c>
@@ -10107,7 +10246,7 @@
         <v>-113.55937376018554</v>
       </c>
     </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A485" t="s">
         <v>3</v>
       </c>
@@ -10127,7 +10266,7 @@
         <v>8.0111087374492627</v>
       </c>
     </row>
-    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A486" t="s">
         <v>0</v>
       </c>
@@ -10147,7 +10286,7 @@
         <v>21.622363963744007</v>
       </c>
     </row>
-    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A487" t="s">
         <v>1</v>
       </c>
@@ -10167,7 +10306,7 @@
         <v>-403.19528794213693</v>
       </c>
     </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A488" t="s">
         <v>2</v>
       </c>
@@ -10187,7 +10326,7 @@
         <v>-15.976439710684531</v>
       </c>
     </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A489" t="s">
         <v>3</v>
       </c>
@@ -10207,7 +10346,7 @@
         <v>217.87163914914396</v>
       </c>
     </row>
-    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A490" t="s">
         <v>0</v>
       </c>
@@ -10227,7 +10366,7 @@
         <v>60.884426404614395</v>
       </c>
     </row>
-    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A491" t="s">
         <v>1</v>
       </c>
@@ -10247,7 +10386,7 @@
         <v>100.37537766655481</v>
       </c>
     </row>
-    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A492" t="s">
         <v>2</v>
       </c>
@@ -10267,7 +10406,7 @@
         <v>330.74434644611955</v>
       </c>
     </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A493" t="s">
         <v>1</v>
       </c>
@@ -10287,7 +10426,7 @@
         <v>-215.47593615527819</v>
       </c>
     </row>
-    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A494" t="s">
         <v>2</v>
       </c>
@@ -10307,7 +10446,7 @@
         <v>-243.84289071321751</v>
       </c>
     </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A495" t="s">
         <v>3</v>
       </c>
@@ -10327,7 +10466,7 @@
         <v>-126.22455519272438</v>
       </c>
     </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A496" t="s">
         <v>0</v>
       </c>
@@ -10347,7 +10486,7 @@
         <v>410.44343394268623</v>
       </c>
     </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A497" t="s">
         <v>1</v>
       </c>
@@ -10367,7 +10506,7 @@
         <v>-139.24069948423721</v>
       </c>
     </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A498" t="s">
         <v>2</v>
       </c>
@@ -10387,7 +10526,7 @@
         <v>-344.12671285134434</v>
       </c>
     </row>
-    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A499" t="s">
         <v>3</v>
       </c>
@@ -10407,7 +10546,7 @@
         <v>-55.925168614764843</v>
       </c>
     </row>
-    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A500" t="s">
         <v>0</v>
       </c>
@@ -10427,7 +10566,7 @@
         <v>1.9989623706778161</v>
       </c>
     </row>
-    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A501" t="s">
         <v>1</v>
       </c>
@@ -10449,10 +10588,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Unknown Document Type" ma:contentTypeID="0x010104" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="05d83ceaa0bbd2e3bc716e6e66bd857a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3d69fe45253d5ff147bb69036b756a7">
     <xsd:element name="properties">
@@ -10566,15 +10718,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -10582,13 +10725,34 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E47F1CCC-34AD-4885-87A9-C94135387DBF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{846CB861-EB1C-4B21-90D5-FBE06079D18B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{846CB861-EB1C-4B21-90D5-FBE06079D18B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E47F1CCC-34AD-4885-87A9-C94135387DBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F28AABEB-2C56-4466-B830-09CA7841A9DA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F28AABEB-2C56-4466-B830-09CA7841A9DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>